<commit_message>
Updated column headers for split _14psticde_type. Updated data dictionary.
</commit_message>
<xml_diff>
--- a/docs/app_data_dictionary.xlsx
+++ b/docs/app_data_dictionary.xlsx
@@ -192,9 +192,6 @@
     <t>3 Knapsack Sprayer (16L)</t>
   </si>
   <si>
-    <t>_14pstcide_type</t>
-  </si>
-  <si>
     <t>Type of pesticide (see pesticide type table)</t>
   </si>
   <si>
@@ -723,7 +720,10 @@
     <t>_14pstcide_type_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Type of pesticide (splitted from _14psticide_type) </t>
+    <t>_14pstcide_type_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of pesticide (splitted from _14psticide_type_1) </t>
   </si>
 </sst>
 </file>
@@ -966,19 +966,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,16 +1283,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1349,161 +1349,161 @@
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" s="35"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1519,16 +1519,16 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1596,39 +1596,39 @@
         <v>45</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1640,7 +1640,7 @@
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1652,7 +1652,7 @@
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1664,19 +1664,19 @@
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="B35" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19" t="s">
-        <v>208</v>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1688,31 +1688,31 @@
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="12" t="s">
         <v>60</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>61</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>65</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1721,98 +1721,98 @@
     </row>
     <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A40" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B40" s="35"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>68</v>
-      </c>
       <c r="C44" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="C45" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>72</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>74</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1821,135 +1821,135 @@
     </row>
     <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A49" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B49" s="35"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B50" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>81</v>
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A61" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B61" s="33"/>
       <c r="C61" s="33"/>
@@ -1957,213 +1957,213 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B64" s="12" t="s">
         <v>99</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>100</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C66" s="19"/>
       <c r="D66" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C68" s="19"/>
       <c r="D68" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B72" s="12" t="s">
         <v>127</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>128</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B73" s="12" t="s">
         <v>129</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>130</v>
       </c>
       <c r="C73" s="19"/>
       <c r="D73" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C74" s="23"/>
       <c r="D74" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B75" s="12" t="s">
         <v>214</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>215</v>
       </c>
       <c r="C75" s="19"/>
       <c r="D75" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B76" s="12" t="s">
         <v>131</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>132</v>
       </c>
       <c r="C76" s="19"/>
       <c r="D76" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B77" s="12" t="s">
         <v>133</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>134</v>
       </c>
       <c r="C77" s="19"/>
       <c r="D77" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B78" s="12" t="s">
         <v>135</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>136</v>
       </c>
       <c r="C78" s="19"/>
       <c r="D78" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A80" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B80" s="35"/>
       <c r="C80" s="35"/>
@@ -2171,57 +2171,57 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B81" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B82" s="12" t="s">
         <v>143</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>144</v>
       </c>
       <c r="C82" s="19"/>
       <c r="D82" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B83" s="12" t="s">
         <v>147</v>
-      </c>
-      <c r="B83" s="12" t="s">
-        <v>148</v>
       </c>
       <c r="C83" s="19"/>
       <c r="D83" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B84" s="12" t="s">
         <v>149</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>150</v>
       </c>
       <c r="C84" s="19"/>
       <c r="D84" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A86" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B86" s="33"/>
       <c r="C86" s="33"/>
@@ -2229,33 +2229,33 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B87" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B88" s="12" t="s">
         <v>152</v>
-      </c>
-      <c r="B88" s="12" t="s">
-        <v>153</v>
       </c>
       <c r="C88" s="19"/>
       <c r="D88" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A90" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B90" s="33"/>
       <c r="C90" s="33"/>
@@ -2263,64 +2263,64 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B91" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C92" s="23"/>
       <c r="D92" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B93" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C93" s="23"/>
       <c r="D93" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="26" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B94" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C94" s="23"/>
       <c r="D94" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C95" s="23"/>
       <c r="D95" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2344,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2357,11 +2357,11 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" s="37"/>
       <c r="D1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2433,7 +2433,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" s="37"/>
     </row>
@@ -2498,7 +2498,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="37"/>
     </row>
@@ -2546,10 +2546,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="B27" s="39"/>
+      <c r="A27" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="42"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -2619,10 +2619,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="40" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="41"/>
+      <c r="A37" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B37" s="40"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -2635,7 +2635,7 @@
         <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2671,10 +2671,10 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="B44" s="39"/>
+      <c r="A44" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="42"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -2721,7 +2721,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B51" s="37"/>
     </row>
@@ -2741,7 +2741,7 @@
         <v>1</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2749,7 +2749,7 @@
         <v>2</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2757,7 +2757,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2770,7 +2770,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="37" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B58" s="37"/>
     </row>
@@ -2790,7 +2790,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2798,7 +2798,7 @@
         <v>2</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2811,7 +2811,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B64" s="37"/>
     </row>
@@ -2831,7 +2831,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2839,7 +2839,7 @@
         <v>2</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2847,7 +2847,7 @@
         <v>3</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2860,7 +2860,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B71" s="37"/>
     </row>
@@ -2880,7 +2880,7 @@
         <v>1</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2888,7 +2888,7 @@
         <v>2</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>3</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2904,7 +2904,7 @@
         <v>4</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2917,7 +2917,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B79" s="37"/>
     </row>
@@ -2937,7 +2937,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2945,7 +2945,7 @@
         <v>2</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2958,7 +2958,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="37" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B85" s="37"/>
     </row>
@@ -2978,7 +2978,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2986,7 +2986,7 @@
         <v>2</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2999,7 +2999,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B91" s="37"/>
     </row>
@@ -3019,7 +3019,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -3027,7 +3027,7 @@
         <v>2</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3035,7 +3035,7 @@
         <v>3</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3048,7 +3048,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B98" s="37"/>
     </row>
@@ -3068,7 +3068,7 @@
         <v>1</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3076,7 +3076,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3084,7 +3084,7 @@
         <v>3</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3097,7 +3097,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B105" s="37"/>
     </row>
@@ -3117,7 +3117,7 @@
         <v>1</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3125,14 +3125,14 @@
         <v>2</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="B110" s="41"/>
+      <c r="A110" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B110" s="40"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
@@ -3145,7 +3145,7 @@
         <v>16</v>
       </c>
       <c r="E111" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3198,7 +3198,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B119" s="37"/>
     </row>
@@ -3218,7 +3218,7 @@
         <v>1</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3226,7 +3226,7 @@
         <v>2</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3234,7 +3234,7 @@
         <v>3</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3242,7 +3242,7 @@
         <v>4</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3250,14 +3250,14 @@
         <v>5</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="42" t="s">
-        <v>175</v>
-      </c>
-      <c r="B127" s="42"/>
+      <c r="A127" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="B127" s="38"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
@@ -3275,7 +3275,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -3283,7 +3283,7 @@
         <v>2</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -3296,11 +3296,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A110:B110"/>
     <mergeCell ref="A91:B91"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:B11"/>
@@ -3314,6 +3309,11 @@
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A110:B110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed unused variables. Removed console.logs. Extracted unique _14pstcide values info ref_pesticide. Created new columns based on _14pstcide_type unique contents (pesticide, herbicide, folia), with values of 0 or 1. Removed non-numerical text in _12freq. Created new _12freq_* columns based on _14pstcide unique values, copied original _12freq value. Updated data dictionary.
</commit_message>
<xml_diff>
--- a/docs/app_data_dictionary.xlsx
+++ b/docs/app_data_dictionary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="243">
   <si>
     <t>_plotno</t>
   </si>
@@ -192,9 +192,6 @@
     <t>3 Knapsack Sprayer (16L)</t>
   </si>
   <si>
-    <t>Type of pesticide (see pesticide type table)</t>
-  </si>
-  <si>
     <t>Pesticide</t>
   </si>
   <si>
@@ -588,9 +585,6 @@
     <t>Weather Station Cell ID</t>
   </si>
   <si>
-    <t>Percentage of P/D occurrence (0=none,1=0-20%; 2=20-40%,…5=80-100%)</t>
-  </si>
-  <si>
     <t>Maximum Temperature (T)</t>
   </si>
   <si>
@@ -717,20 +711,79 @@
     <t>Date (yyyy-mm-dd), but defaults to (mm/dd/yyyy) when opened in Excel</t>
   </si>
   <si>
-    <t>_14pstcide_type_1</t>
-  </si>
-  <si>
-    <t>_14pstcide_type_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of pesticide (splitted from _14psticide_type_1) </t>
+    <t>_14pstcide_type_herbicide</t>
+  </si>
+  <si>
+    <t>_14pstcide_type_pesticide</t>
+  </si>
+  <si>
+    <t>_14pstcide_type_folia</t>
+  </si>
+  <si>
+    <t>_12freq_folia</t>
+  </si>
+  <si>
+    <t>_12freq_herbicide</t>
+  </si>
+  <si>
+    <t>_12freq_pesticide</t>
+  </si>
+  <si>
+    <t>Pesticide frequency rate for folia (see pesticide frequency rate table)</t>
+  </si>
+  <si>
+    <t>Pesticide frequency rate for herbicide (see pesticide frequency rate table)</t>
+  </si>
+  <si>
+    <t>Pesticide frequency rate for pesticide(see pesticide frequency rate table)</t>
+  </si>
+  <si>
+    <t>_14pstcide_type</t>
+  </si>
+  <si>
+    <t>Type of pesticide, excluded from output. May contain "folia, pesticide or herbicide" text values. (see pesticide type table for values)</t>
+  </si>
+  <si>
+    <t>Type of pesticide: folia derived from values of _14pstcide type (see pesticide type table)</t>
+  </si>
+  <si>
+    <t>Type of pesticide: herbicide derived from values of _14pstcide type (see pesticide type table)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of pesticide: pesticide derived from values of_14pstcide type (splitted from _14psticide_type_1) </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Percentage of P/D occurrence (0=none,1=0-20%; 2=20-40%,…5=80-100%). </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A value of 0 does not denote the absence of P&amp;D because the farmer may not recall the % of damage, but has observed prescence of other pest or disease variables.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -762,6 +815,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -857,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -950,6 +1011,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1261,38 +1328,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="3" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="67.140625" style="13" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" style="18" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="35"/>
+      <c r="B1" s="37"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1304,7 +1372,7 @@
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1316,7 +1384,7 @@
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,7 +1396,7 @@
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1340,7 +1408,7 @@
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1348,162 +1416,162 @@
       <c r="D7" s="21"/>
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="35"/>
+      <c r="A8" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="37"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="B10" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24" t="s">
         <v>203</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="21" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C11" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>204</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C12" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>204</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C13" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" s="21" t="s">
         <v>204</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="29" t="s">
         <v>216</v>
       </c>
-      <c r="B20" s="29" t="s">
-        <v>218</v>
-      </c>
       <c r="C20" s="30" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1512,23 +1580,23 @@
       <c r="D21" s="21"/>
     </row>
     <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="37"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1540,7 +1608,7 @@
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1552,7 +1620,7 @@
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1564,7 +1632,7 @@
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1576,7 +1644,7 @@
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1588,7 +1656,7 @@
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1596,39 +1664,39 @@
         <v>45</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>200</v>
-      </c>
       <c r="C30" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>201</v>
-      </c>
       <c r="C31" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1640,10 +1708,10 @@
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
@@ -1652,687 +1720,747 @@
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>55</v>
+        <v>235</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="23" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="23" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="19" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="19"/>
-      <c r="D39" s="21"/>
-    </row>
-    <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="35"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>215</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="B38" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>209</v>
+        <v>58</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>211</v>
+        <v>59</v>
       </c>
       <c r="C42" s="19"/>
-      <c r="D42" s="21" t="s">
-        <v>207</v>
+      <c r="D42" s="19" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>210</v>
+        <v>62</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>212</v>
+        <v>63</v>
       </c>
       <c r="C43" s="19"/>
-      <c r="D43" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>207</v>
-      </c>
+      <c r="D43" s="19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="19"/>
+      <c r="D44" s="21"/>
+    </row>
+    <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="37"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="21" t="s">
-        <v>207</v>
+      <c r="A46" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>72</v>
+        <v>207</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>73</v>
+        <v>209</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>210</v>
+      </c>
       <c r="C48" s="19"/>
-      <c r="D48" s="21"/>
-    </row>
-    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" s="35"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>82</v>
-      </c>
       <c r="C53" s="19"/>
-      <c r="D53" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="21" t="s">
-        <v>207</v>
-      </c>
+      <c r="D53" s="21"/>
+    </row>
+    <row r="54" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="37"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="B61" s="33"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>215</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" s="19"/>
+      <c r="D60" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="19"/>
+      <c r="D61" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="19"/>
+      <c r="D62" s="21" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>155</v>
+        <v>79</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C66" s="19"/>
-      <c r="D66" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C67" s="19"/>
-      <c r="D67" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" s="35"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="35"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="C68" s="19"/>
       <c r="D68" s="21" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C73" s="19"/>
       <c r="D73" s="21" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="B74" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="C74" s="23"/>
-      <c r="D74" s="24" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" s="19"/>
+      <c r="D74" s="21" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>213</v>
+        <v>120</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>214</v>
+        <v>122</v>
       </c>
       <c r="C75" s="19"/>
       <c r="D75" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C76" s="19"/>
       <c r="D76" s="21" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C77" s="19"/>
       <c r="D77" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C78" s="19"/>
       <c r="D78" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="B80" s="35"/>
-      <c r="C80" s="35"/>
-      <c r="D80" s="36"/>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B79" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="C79" s="23"/>
+      <c r="D79" s="24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C80" s="19"/>
+      <c r="D80" s="21" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="D81" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" s="19"/>
+      <c r="D81" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C82" s="19"/>
       <c r="D82" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="C83" s="19"/>
       <c r="D83" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C84" s="19"/>
-      <c r="D84" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="B86" s="33"/>
-      <c r="C86" s="33"/>
-      <c r="D86" s="33"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B87" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B85" s="37"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="38"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B86" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C87" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="D87" s="17" t="s">
-        <v>215</v>
+      <c r="C86" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C87" s="19"/>
+      <c r="D87" s="21" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C88" s="19"/>
       <c r="D88" s="21" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="33" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C89" s="19"/>
+      <c r="D89" s="21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="B91" s="35"/>
+      <c r="C91" s="35"/>
+      <c r="D91" s="35"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C93" s="19"/>
+      <c r="D93" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="B95" s="35"/>
+      <c r="C95" s="35"/>
+      <c r="D95" s="35"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D96" s="17" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B97" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="C97" s="23"/>
+      <c r="D97" s="24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="B90" s="33"/>
-      <c r="C90" s="33"/>
-      <c r="D90" s="33"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B91" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="D91" s="17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="B92" s="27" t="s">
+      <c r="B98" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C98" s="23"/>
+      <c r="D98" s="24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="C92" s="23"/>
-      <c r="D92" s="24" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="B93" s="27" t="s">
+      <c r="B99" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="C99" s="23"/>
+      <c r="D99" s="24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="C93" s="23"/>
-      <c r="D93" s="24" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="26" t="s">
-        <v>225</v>
-      </c>
-      <c r="B94" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="C94" s="23"/>
-      <c r="D94" s="24" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="26" t="s">
+      <c r="B100" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="B95" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="C95" s="23"/>
-      <c r="D95" s="24" t="s">
-        <v>207</v>
+      <c r="C100" s="23"/>
+      <c r="D100" s="24" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A66:D66"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A54:B54"/>
     <mergeCell ref="A8:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2344,8 +2472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2356,12 +2484,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="37"/>
+      <c r="A1" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="39"/>
       <c r="D1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2432,10 +2560,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11" s="37"/>
+      <c r="A11" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="39"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -2497,10 +2625,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="37" t="s">
-        <v>161</v>
-      </c>
-      <c r="B20" s="37"/>
+      <c r="A20" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="39"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -2546,10 +2674,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27" s="42"/>
+      <c r="A27" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" s="44"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -2619,10 +2747,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37" s="42"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -2635,7 +2763,7 @@
         <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2671,10 +2799,10 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="B44" s="42"/>
+      <c r="A44" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="44"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -2720,10 +2848,10 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="B51" s="37"/>
+      <c r="A51" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" s="39"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
@@ -2741,7 +2869,7 @@
         <v>1</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2749,7 +2877,7 @@
         <v>2</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2757,7 +2885,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2769,10 +2897,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="37" t="s">
-        <v>165</v>
-      </c>
-      <c r="B58" s="37"/>
+      <c r="A58" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" s="39"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
@@ -2790,7 +2918,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2798,7 +2926,7 @@
         <v>2</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2810,10 +2938,10 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="B64" s="37"/>
+      <c r="A64" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="B64" s="39"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
@@ -2831,7 +2959,7 @@
         <v>1</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2839,7 +2967,7 @@
         <v>2</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2847,7 +2975,7 @@
         <v>3</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2859,10 +2987,10 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="37" t="s">
-        <v>167</v>
-      </c>
-      <c r="B71" s="37"/>
+      <c r="A71" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="B71" s="39"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
@@ -2880,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2888,7 +3016,7 @@
         <v>2</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2896,7 +3024,7 @@
         <v>3</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2904,7 +3032,7 @@
         <v>4</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2916,10 +3044,10 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="B79" s="37"/>
+      <c r="A79" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="B79" s="39"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
@@ -2937,7 +3065,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2945,7 +3073,7 @@
         <v>2</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2957,10 +3085,10 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="B85" s="37"/>
+      <c r="A85" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="39"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
@@ -2978,7 +3106,7 @@
         <v>1</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2986,7 +3114,7 @@
         <v>2</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2998,10 +3126,10 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="B91" s="37"/>
+      <c r="A91" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="B91" s="39"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
@@ -3019,7 +3147,7 @@
         <v>1</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -3027,7 +3155,7 @@
         <v>2</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3035,7 +3163,7 @@
         <v>3</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3047,10 +3175,10 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="37" t="s">
-        <v>171</v>
-      </c>
-      <c r="B98" s="37"/>
+      <c r="A98" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="B98" s="39"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
@@ -3068,7 +3196,7 @@
         <v>1</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3076,7 +3204,7 @@
         <v>2</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3084,7 +3212,7 @@
         <v>3</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3096,10 +3224,10 @@
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="B105" s="37"/>
+      <c r="A105" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="B105" s="39"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
@@ -3117,7 +3245,7 @@
         <v>1</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3125,14 +3253,14 @@
         <v>2</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="B110" s="40"/>
+      <c r="A110" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="B110" s="42"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
@@ -3145,7 +3273,7 @@
         <v>16</v>
       </c>
       <c r="E111" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3197,10 +3325,10 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="B119" s="37"/>
+      <c r="A119" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="B119" s="39"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
@@ -3218,7 +3346,7 @@
         <v>1</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3226,7 +3354,7 @@
         <v>2</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3234,7 +3362,7 @@
         <v>3</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3242,7 +3370,7 @@
         <v>4</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3250,14 +3378,14 @@
         <v>5</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="B127" s="38"/>
+      <c r="A127" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="B127" s="40"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
@@ -3275,7 +3403,7 @@
         <v>1</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -3283,7 +3411,7 @@
         <v>2</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated data dictionary to 4.0.
</commit_message>
<xml_diff>
--- a/docs/app_data_dictionary.xlsx
+++ b/docs/app_data_dictionary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="255">
   <si>
     <t>_plotno</t>
   </si>
@@ -591,15 +591,9 @@
     <t>Minimum Temperature (T)</t>
   </si>
   <si>
-    <t>average of Tmax and Tmin</t>
-  </si>
-  <si>
     <t>Diurned range</t>
   </si>
   <si>
-    <t>frequency of days with Tmax &gt;= 31 degrees Celsius</t>
-  </si>
-  <si>
     <t>Precipitation accumulated; monthly total of Precipitation (P)</t>
   </si>
   <si>
@@ -670,9 +664,6 @@
   </si>
   <si>
     <t>w_growthstg_date</t>
-  </si>
-  <si>
-    <t>11_growthstg_clean</t>
   </si>
   <si>
     <t>Date where PD was observed (_07pdate + _11growthstg_clean)</t>
@@ -779,9 +770,6 @@
     </r>
   </si>
   <si>
-    <t>Version 3.0.0</t>
-  </si>
-  <si>
     <t>_14pstcide_type_foliar</t>
   </si>
   <si>
@@ -801,13 +789,60 @@
   </si>
   <si>
     <t>Frequency rate of _14pstcide_type_pesticide (if any)</t>
+  </si>
+  <si>
+    <t>NOTE:</t>
+  </si>
+  <si>
+    <t>Weather variables can be appended with an integer (i.e., 30w_tmax, 30w_tmin, 30w_tavg,…) where the integer 30 represents the number of days backtracked from the w_growthsg_date.</t>
+  </si>
+  <si>
+    <t>_11growthstg_clean</t>
+  </si>
+  <si>
+    <t>Version 4.0.0</t>
+  </si>
+  <si>
+    <t>Average of Tmax and Tmin</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Frequency of days with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tmax &gt;= 31</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> degrees Celsius</t>
+    </r>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>random firebase key</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,7 +873,9 @@
       <scheme val="major"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -846,13 +883,27 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -867,18 +918,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -938,11 +1025,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -967,9 +1067,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -982,12 +1079,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1003,74 +1094,167 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1352,1195 +1536,1218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="67.140625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="67.140625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="15" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="B1" s="37"/>
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="34"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19" t="s">
-        <v>203</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="21" t="s">
-        <v>205</v>
+      <c r="C6" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="21" t="s">
-        <v>205</v>
+      <c r="C7" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="21" t="s">
-        <v>205</v>
+      <c r="C8" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="19"/>
-      <c r="D9" s="21"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="51"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="68" t="s">
         <v>183</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="69" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>242</v>
-      </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24" t="s">
-        <v>203</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="67" t="s">
         <v>175</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="D13" s="21" t="s">
-        <v>204</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="70" t="s">
         <v>176</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="D14" s="21" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="70" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="70" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="70" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="70" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="70" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="70" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="27"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="D24" s="26"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="D25" s="26"/>
+    </row>
+    <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="C15" s="19" t="s">
+      <c r="D34" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="D15" s="21" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="67" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="D35" s="18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="69" t="s">
+        <v>228</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="69" t="s">
+        <v>229</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="69" t="s">
+        <v>230</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="69" t="s">
+        <v>234</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="69" t="s">
+        <v>227</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="31"/>
+      <c r="B48" s="32"/>
+      <c r="D48" s="26"/>
+    </row>
+    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" s="46"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="47"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="D50" s="44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C51" s="16"/>
+      <c r="D51" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="67" t="s">
+        <v>206</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="C52" s="16"/>
+      <c r="D52" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="16"/>
+      <c r="D55" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" s="16"/>
+      <c r="D56" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="31"/>
+      <c r="B57" s="32"/>
+      <c r="D57" s="26"/>
+    </row>
+    <row r="58" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" s="53"/>
+      <c r="C58" s="53"/>
+      <c r="D58" s="54"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="D59" s="44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="16"/>
+      <c r="D60" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="16"/>
+      <c r="D61" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" s="16"/>
+      <c r="D62" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="16"/>
+      <c r="D63" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="16"/>
+      <c r="D64" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" s="16"/>
+      <c r="D65" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="16"/>
+      <c r="D66" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="16"/>
+      <c r="D67" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" s="16"/>
+      <c r="D68" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="56"/>
+      <c r="C70" s="56"/>
+      <c r="D70" s="57"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B71" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="D71" s="44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C72" s="16"/>
+      <c r="D72" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C73" s="16"/>
+      <c r="D73" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C74" s="16"/>
+      <c r="D74" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C75" s="16"/>
+      <c r="D75" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="67" t="s">
+        <v>105</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C76" s="16"/>
+      <c r="D76" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C77" s="16"/>
+      <c r="D77" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C78" s="16"/>
+      <c r="D78" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="67" t="s">
+        <v>120</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" s="16"/>
+      <c r="D79" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" s="16"/>
+      <c r="D80" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" s="16"/>
+      <c r="D81" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" s="16"/>
+      <c r="D82" s="18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="72" t="s">
+        <v>249</v>
+      </c>
+      <c r="B83" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="C83" s="17"/>
+      <c r="D83" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="67" t="s">
+        <v>209</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C84" s="16"/>
+      <c r="D84" s="18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C85" s="16"/>
+      <c r="D85" s="18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="67" t="s">
+        <v>131</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C86" s="16"/>
+      <c r="D86" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C87" s="16"/>
+      <c r="D87" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89" s="59"/>
+      <c r="C89" s="59"/>
+      <c r="D89" s="60"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B90" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="D90" s="44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C91" s="16"/>
+      <c r="D91" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="67" t="s">
+        <v>145</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C92" s="16"/>
+      <c r="D92" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C93" s="16"/>
+      <c r="D93" s="18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="B95" s="62"/>
+      <c r="C95" s="62"/>
+      <c r="D95" s="63"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B96" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="D96" s="44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="B97" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C97" s="16"/>
+      <c r="D97" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="64" t="s">
+        <v>215</v>
+      </c>
+      <c r="B99" s="65"/>
+      <c r="C99" s="65"/>
+      <c r="D99" s="66"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="B100" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="D100" s="44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="69" t="s">
         <v>216</v>
       </c>
-      <c r="C22" s="30" t="s">
-        <v>227</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="21"/>
-    </row>
-    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="37"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="17" t="s">
+      <c r="B101" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="C101" s="17"/>
+      <c r="D101" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="69" t="s">
+        <v>217</v>
+      </c>
+      <c r="B102" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C102" s="17"/>
+      <c r="D102" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="69" t="s">
+        <v>220</v>
+      </c>
+      <c r="B103" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C103" s="17"/>
+      <c r="D103" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="69" t="s">
+        <v>221</v>
+      </c>
+      <c r="B104" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="C104" s="17"/>
+      <c r="D104" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="67" t="s">
+        <v>240</v>
+      </c>
+      <c r="B105" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="C105" s="16"/>
+      <c r="D105" s="18" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B106" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="C106" s="16"/>
+      <c r="D106" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="B38" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
-        <v>237</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+    </row>
+    <row r="107" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C107" s="16"/>
+      <c r="D107" s="18" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B41" s="27" t="s">
-        <v>239</v>
-      </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
-        <v>228</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="B43" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="19"/>
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B47" s="37"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="17" t="s">
+      <c r="B108" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C108" s="16"/>
+      <c r="D108" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="D48" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C49" s="19"/>
-      <c r="D49" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="D51" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="D52" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="19"/>
-      <c r="D55" s="21"/>
-    </row>
-    <row r="56" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="B56" s="37"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C58" s="19"/>
-      <c r="D58" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C59" s="19"/>
-      <c r="D59" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C60" s="19"/>
-      <c r="D60" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="19"/>
-      <c r="D61" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C62" s="19"/>
-      <c r="D62" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C63" s="19"/>
-      <c r="D63" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C66" s="19"/>
-      <c r="D66" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="C70" s="19"/>
-      <c r="D70" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B71" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="C71" s="19"/>
-      <c r="D71" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B72" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C72" s="19"/>
-      <c r="D72" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C73" s="19"/>
-      <c r="D73" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C74" s="19"/>
-      <c r="D74" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C75" s="19"/>
-      <c r="D75" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B76" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" s="19"/>
-      <c r="D76" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B77" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C77" s="19"/>
-      <c r="D77" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B78" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C78" s="19"/>
-      <c r="D78" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B79" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C79" s="19"/>
-      <c r="D79" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B80" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C80" s="19"/>
-      <c r="D80" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B81" s="25" t="s">
-        <v>217</v>
-      </c>
-      <c r="C81" s="23"/>
-      <c r="D81" s="24" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C82" s="19"/>
-      <c r="D82" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B83" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C83" s="19"/>
-      <c r="D83" s="21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B84" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C84" s="19"/>
-      <c r="D84" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B85" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C85" s="19"/>
-      <c r="D85" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="B87" s="37"/>
-      <c r="C87" s="37"/>
-      <c r="D87" s="38"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="D88" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B89" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C89" s="19"/>
-      <c r="D89" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B90" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C90" s="19"/>
-      <c r="D90" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B91" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C91" s="19"/>
-      <c r="D91" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="35" t="s">
-        <v>149</v>
-      </c>
-      <c r="B93" s="35"/>
-      <c r="C93" s="35"/>
-      <c r="D93" s="35"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="D94" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B95" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C95" s="19"/>
-      <c r="D95" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="B97" s="35"/>
-      <c r="C97" s="35"/>
-      <c r="D97" s="35"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B98" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C98" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="D98" s="17" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="B99" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="C99" s="23"/>
-      <c r="D99" s="24" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="26" t="s">
-        <v>220</v>
-      </c>
-      <c r="B100" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="C100" s="23"/>
-      <c r="D100" s="24" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="26" t="s">
-        <v>223</v>
-      </c>
-      <c r="B101" s="27" t="s">
-        <v>225</v>
-      </c>
-      <c r="C101" s="23"/>
-      <c r="D101" s="24" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="B102" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="C102" s="23"/>
-      <c r="D102" s="24" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="B103" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="C103" s="19"/>
-      <c r="D103" s="21" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="B104" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="C104" s="19"/>
-      <c r="D104" s="21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B105" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="C105" s="19"/>
-      <c r="D105" s="21" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="B106" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="C106" s="19"/>
-      <c r="D106" s="21" t="s">
-        <v>203</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2563,10 +2770,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="B1" s="39"/>
+      <c r="B1" s="20"/>
       <c r="D1" s="1" t="s">
         <v>155</v>
       </c>
@@ -2639,10 +2846,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B11" s="39"/>
+      <c r="B11" s="20"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -2704,10 +2911,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="B20" s="39"/>
+      <c r="B20" s="20"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -2753,10 +2960,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="B27" s="41"/>
+      <c r="B27" s="25"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -2826,10 +3033,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="B37" s="43"/>
+      <c r="B37" s="23"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -2878,10 +3085,10 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="B44" s="41"/>
+      <c r="B44" s="25"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -2927,10 +3134,10 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="39" t="s">
+      <c r="A51" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B51" s="39"/>
+      <c r="B51" s="20"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
@@ -2976,10 +3183,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="B58" s="39"/>
+      <c r="B58" s="20"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
@@ -3017,10 +3224,10 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="39" t="s">
+      <c r="A64" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B64" s="39"/>
+      <c r="B64" s="20"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
@@ -3066,10 +3273,10 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="39" t="s">
+      <c r="A71" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="B71" s="39"/>
+      <c r="B71" s="20"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
@@ -3123,10 +3330,10 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="39" t="s">
+      <c r="A79" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="B79" s="39"/>
+      <c r="B79" s="20"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
@@ -3164,10 +3371,10 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="39" t="s">
+      <c r="A85" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="39"/>
+      <c r="B85" s="20"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
@@ -3205,10 +3412,10 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="39" t="s">
+      <c r="A91" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="B91" s="39"/>
+      <c r="B91" s="20"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
@@ -3254,10 +3461,10 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="39" t="s">
+      <c r="A98" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="B98" s="39"/>
+      <c r="B98" s="20"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
@@ -3303,10 +3510,10 @@
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="39" t="s">
+      <c r="A105" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B105" s="39"/>
+      <c r="B105" s="20"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
@@ -3336,10 +3543,10 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="42" t="s">
+      <c r="A110" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="B110" s="43"/>
+      <c r="B110" s="23"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
@@ -3404,10 +3611,10 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="39" t="s">
+      <c r="A119" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="B119" s="39"/>
+      <c r="B119" s="20"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
@@ -3461,10 +3668,10 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="44" t="s">
+      <c r="A127" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="B127" s="44"/>
+      <c r="B127" s="21"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
@@ -3503,11 +3710,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A110:B110"/>
     <mergeCell ref="A91:B91"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:B11"/>
@@ -3521,6 +3723,11 @@
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A110:B110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>